<commit_message>
Actualizamos modulo de arquitctos
</commit_message>
<xml_diff>
--- a/Arquitectos.xlsx
+++ b/Arquitectos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2018\Desarrollo_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2018\Desarrollo_cpnaa\cpnaa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nombres</t>
   </si>
@@ -48,42 +48,6 @@
   </si>
   <si>
     <t>Cedula_RL</t>
-  </si>
-  <si>
-    <t>Angelica</t>
-  </si>
-  <si>
-    <t>Roma</t>
-  </si>
-  <si>
-    <t>cr@gmail.com</t>
-  </si>
-  <si>
-    <t>profesional</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Jimenez</t>
-  </si>
-  <si>
-    <t>juan@gmail.com</t>
-  </si>
-  <si>
-    <t>auxiliar</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>mendez</t>
-  </si>
-  <si>
-    <t>maria@gmail.com</t>
-  </si>
-  <si>
-    <t>tecnico</t>
   </si>
 </sst>
 </file>
@@ -417,7 +381,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,89 +416,15 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>42568759</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>7730351</v>
-      </c>
-      <c r="F2">
-        <v>979879798</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>1015451163</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>32154689</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>87954213</v>
-      </c>
-      <c r="F3">
-        <v>879546546</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>1015451163</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>2135468</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>5789542</v>
-      </c>
-      <c r="F4">
-        <v>89789546213</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4">
-        <v>1015451163</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizamos proyecto con los cambios solicitados por el cliente, se modifica datos de session y subida de excel, cambios en administración y en vista de usuario.
</commit_message>
<xml_diff>
--- a/Arquitectos.xlsx
+++ b/Arquitectos.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2018\Desarrollo_cpnaa\cpnaa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Desarrollo_cpnaa\cpnaa\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD80395-F406-45E2-BF20-65B771C15068}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8835" windowHeight="3330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8835" windowHeight="3330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombres</t>
   </si>
@@ -41,19 +43,22 @@
     <t>Telefono</t>
   </si>
   <si>
-    <t>Nit_empresa</t>
-  </si>
-  <si>
     <t>Nivel_educativo</t>
   </si>
   <si>
-    <t>Cedula_RL</t>
+    <t>Arquitecto/a</t>
+  </si>
+  <si>
+    <t>Técnico/a</t>
+  </si>
+  <si>
+    <t>Tecnólogo/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,19 +382,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,21 +415,57 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{800A24E3-FD0B-4978-8F9F-433DB8090215}">
+          <x14:formula1>
+            <xm:f>Hoja2!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F500</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B8BC3B-7780-4E35-8072-23035A869BC4}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>